<commit_message>
Fixed bugs with the new format
</commit_message>
<xml_diff>
--- a/rates.xlsx
+++ b/rates.xlsx
@@ -377,7 +377,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B205"/>
+  <dimension ref="A1:B206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2023,6 +2023,14 @@
         <v>34006993.7229999</v>
       </c>
     </row>
+    <row r="206" spans="1:2">
+      <c r="A206">
+        <v>202008</v>
+      </c>
+      <c r="B206">
+        <v>34006993.7229999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>